<commit_message>
Updated with 4 robots and it's working good
Need to clean code and add proper comments
</commit_message>
<xml_diff>
--- a/Versions.xlsx
+++ b/Versions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Version</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Transverse entire arena</t>
+  </si>
+  <si>
+    <t>Current</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -620,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -649,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -658,6 +661,35 @@
         <v>1</v>
       </c>
       <c r="I9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>